<commit_message>
Registrar Usuario - fin con fallos
Se finaliza la función añadir fallos, quedando pendientes de corregir fallos, relativos al posterior login del cliente añadido
</commit_message>
<xml_diff>
--- a/BaseDeDatosUsuarios.xlsx
+++ b/BaseDeDatosUsuarios.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotace\Desktop\HealthApp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115C7811-1BFD-481E-8246-3BE913B53CF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -55,28 +49,49 @@
     <t>tipo</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>jesus</t>
   </si>
   <si>
+    <t>Guille</t>
+  </si>
+  <si>
+    <t>Fulano</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
     <t>carro</t>
   </si>
   <si>
+    <t>Calvo</t>
+  </si>
+  <si>
+    <t>Fulanito</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
     <t>H</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
     <t>subir</t>
-  </si>
-  <si>
-    <t>Guille</t>
-  </si>
-  <si>
-    <t>Calvo</t>
-  </si>
-  <si>
-    <t>Fulano</t>
-  </si>
-  <si>
-    <t>Fulanito</t>
   </si>
   <si>
     <t>mantener</t>
@@ -85,8 +100,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,19 +164,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -203,7 +210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,27 +242,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,24 +276,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,16 +451,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,21 +493,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>71308125</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -547,7 +516,7 @@
         <v>178</v>
       </c>
       <c r="H2">
-        <v>73.400000000000006</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -556,24 +525,24 @@
         <v>-1</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1234</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1234</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F3">
         <v>21</v>
@@ -591,15 +560,15 @@
         <v>-1</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -608,7 +577,7 @@
         <v>1234</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>32</v>
@@ -626,7 +595,42 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadir Alimento 2.0 - Inicio
Se modifica el Añadir alimento para implementar la metodología ntriscore al sistema de alimentos.
</commit_message>
<xml_diff>
--- a/BaseDeDatosUsuarios.xlsx
+++ b/BaseDeDatosUsuarios.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\Desktop\TFG\HealhApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA26905-7E1F-4BA8-8750-2B79E45D576D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -49,16 +55,13 @@
     <t>tipo</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>jesus</t>
   </si>
   <si>
     <t>Guille</t>
   </si>
   <si>
-    <t>Fulano</t>
+    <t>Juanjo</t>
   </si>
   <si>
     <t>Ana</t>
@@ -70,7 +73,7 @@
     <t>Calvo</t>
   </si>
   <si>
-    <t>Fulanito</t>
+    <t>Juanjito</t>
   </si>
   <si>
     <t>Perez</t>
@@ -82,16 +85,10 @@
     <t>M</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>168</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
     <t>subir</t>
+  </si>
+  <si>
+    <t>bajar</t>
   </si>
   <si>
     <t>mantener</t>
@@ -100,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,11 +161,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -210,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,9 +247,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,6 +299,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,14 +492,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="A6:K6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,21 +536,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>71308125</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1234</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -516,7 +559,7 @@
         <v>178</v>
       </c>
       <c r="H2">
-        <v>73.40000000000001</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -525,24 +568,24 @@
         <v>-1</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1234</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>1234</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <v>21</v>
@@ -560,68 +603,68 @@
         <v>-1</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>1234</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="G4">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H4">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>11</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
       </c>
       <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
+      <c r="G5">
+        <v>168</v>
+      </c>
+      <c r="H5">
+        <v>55</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -630,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>